<commit_message>
fixed close not including ncv
</commit_message>
<xml_diff>
--- a/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplatesTempFolder/2019-09-18_RBU_PROOF_SHEET.xlsx
+++ b/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplatesTempFolder/2019-09-18_RBU_PROOF_SHEET.xlsx
@@ -2515,12 +2515,12 @@
       <c r="N26" s="103"/>
       <c r="O26" s="104"/>
       <c r="P26" s="114">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="Q26" s="115"/>
       <c r="R26" s="116"/>
       <c r="S26" s="117">
-        <v>14634325.58</v>
+        <v>14772381.58</v>
       </c>
       <c r="T26" s="118"/>
       <c r="U26" s="118"/>
@@ -3648,12 +3648,12 @@
       <c r="N51" s="25"/>
       <c r="O51" s="26"/>
       <c r="P51" s="24">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="Q51" s="25"/>
       <c r="R51" s="26"/>
       <c r="S51" s="32">
-        <v>14634325.58</v>
+        <v>14772381.58</v>
       </c>
       <c r="T51" s="33"/>
       <c r="U51" s="33"/>

</xml_diff>